<commit_message>
added form-validation + formatted code
</commit_message>
<xml_diff>
--- a/Peiling.xlsx
+++ b/Peiling.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gijsd\WebstormProjects\peilingen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G.deLange\Documents\GitHub\peilingen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E6A4E6-FC6C-4354-92EC-50BA0AC6A941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD6AF8B-1034-4974-B478-9200F1BF5876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{F860C830-3069-4E45-9470-11FABD2A9123}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F860C830-3069-4E45-9470-11FABD2A9123}"/>
   </bookViews>
   <sheets>
-    <sheet name="Verian" sheetId="1" r:id="rId1"/>
-    <sheet name="Maurice de Hond" sheetId="2" r:id="rId2"/>
+    <sheet name="Maurice de Hond" sheetId="2" r:id="rId1"/>
+    <sheet name="Verian" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -161,7 +161,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -177,7 +177,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -492,10 +492,154 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F5C7F7-8573-4525-B5B3-D286C9BADC47}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9:XFD9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A25611E-F488-44A3-8FFA-40CC2E44D187}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
@@ -637,148 +781,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F5C7F7-8573-4525-B5B3-D286C9BADC47}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:XFD9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="1">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>